<commit_message>
update the calculation of upper bound of heat exchange between hot and cold streams.
</commit_message>
<xml_diff>
--- a/hens/test_case.xlsx
+++ b/hens/test_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\may3r\PycharmProjects\COSMO\hens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B28E78-9FE7-4415-817F-ADFE6B1BD7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D4C4A7-193B-4D49-A7F6-BA9073886DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="1612" windowWidth="30045" windowHeight="17093" xr2:uid="{55A3D58C-627B-4C9F-A3AC-B99D6961FBEF}"/>
+    <workbookView xWindow="19118" yWindow="0" windowWidth="19365" windowHeight="20963" xr2:uid="{55A3D58C-627B-4C9F-A3AC-B99D6961FBEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{3A896AD7-4125-4BEC-87EF-D4193813A363}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -591,26 +591,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6460,12 +6440,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E70EA7A-D1DD-4AB3-B1A7-7C3340032068}" name="Table3" displayName="Table3" ref="A2:F22" totalsRowShown="0">
   <autoFilter ref="A2:F22" xr:uid="{5282843C-0FDD-C940-ABEB-01C7BA357338}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{51161E5C-B970-4A5B-8104-33DD52FA0EF6}" name="Stream no" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{51161E5C-B970-4A5B-8104-33DD52FA0EF6}" name="Stream no" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{71E0C6C2-353E-41AC-B4DB-82579879651E}" name="Stream Name"/>
-    <tableColumn id="3" xr3:uid="{BAED1916-3B93-426B-8D2C-3C3D00DDDA30}" name="Supply Temp" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{F2FA5C5B-2BC4-4460-8649-C7005BB98E94}" name="Target Temp" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{4EC3CF15-387C-4C65-832E-C5CEE8106FE1}" name="Heat Cap" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{FDD9F0D0-850A-4715-B314-5C921BF0C69A}" name="Enthalpy change" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{BAED1916-3B93-426B-8D2C-3C3D00DDDA30}" name="Supply Temp" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F2FA5C5B-2BC4-4460-8649-C7005BB98E94}" name="Target Temp" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{4EC3CF15-387C-4C65-832E-C5CEE8106FE1}" name="Heat Cap" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{FDD9F0D0-850A-4715-B314-5C921BF0C69A}" name="Enthalpy change" dataDxfId="6">
       <calculatedColumnFormula>IF(Table3[[#This Row],[Heat Cap]],ABS(Table3[[#This Row],[Target Temp]]-Table3[[#This Row],[Supply Temp]])*Table3[[#This Row],[Heat Cap]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6477,12 +6457,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09A6D4DF-E638-4138-8EF0-4D8D308F4C4E}" name="Table4" displayName="Table4" ref="H2:M22" totalsRowShown="0">
   <autoFilter ref="H2:M22" xr:uid="{C2819A13-B954-F744-A937-195205D73C92}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{ECA15CAA-9B7C-4CA8-9A92-76A96085E693}" name="Stream no" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{ECA15CAA-9B7C-4CA8-9A92-76A96085E693}" name="Stream no" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{C7FD695F-4DD9-480C-9BE7-CBF936487862}" name="Stream Name"/>
-    <tableColumn id="3" xr3:uid="{6B08F010-5BE0-469A-AFEC-401DEFAC2BC2}" name="Supply Temp" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{6DAB91F0-ABCB-4103-A612-B4CB15012200}" name="Target Temp" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{9C848C1C-BC49-4229-916A-1B024467F3FA}" name="Heat Cap" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{CB901371-BCA9-417B-9021-899661F2CBCF}" name="Enthalpy change" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{6B08F010-5BE0-469A-AFEC-401DEFAC2BC2}" name="Supply Temp" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{6DAB91F0-ABCB-4103-A612-B4CB15012200}" name="Target Temp" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{9C848C1C-BC49-4229-916A-1B024467F3FA}" name="Heat Cap" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CB901371-BCA9-417B-9021-899661F2CBCF}" name="Enthalpy change" dataDxfId="1">
       <calculatedColumnFormula>IF(Table4[[#This Row],[Heat Cap]],ABS(Table4[[#This Row],[Target Temp]]-Table4[[#This Row],[Supply Temp]])*Table4[[#This Row],[Heat Cap]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6817,8 +6797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D46D52-B92F-4C13-90EE-CFC876B09C87}">
   <dimension ref="A2:BD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX14" sqref="AX14:BD22"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP68" sqref="AP68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.4"/>
@@ -6894,7 +6874,7 @@
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="X3" t="s">
         <v>3</v>
@@ -6918,7 +6898,7 @@
         <v>1</v>
       </c>
       <c r="AG3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AH3" t="s">
         <v>3</v>
@@ -6930,7 +6910,7 @@
         <v>5</v>
       </c>
       <c r="AK3" s="1">
-        <v>147.4</v>
+        <v>82.9</v>
       </c>
       <c r="AL3" t="s">
         <v>25</v>
@@ -6998,7 +6978,7 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="N4" t="s">
         <v>3</v>
@@ -7010,7 +6990,7 @@
         <v>5</v>
       </c>
       <c r="Q4" s="1">
-        <v>1159.2</v>
+        <v>625.6</v>
       </c>
       <c r="U4" t="s">
         <v>0</v>
@@ -7052,7 +7032,7 @@
         <v>5</v>
       </c>
       <c r="AK4" s="1">
-        <v>228.9</v>
+        <v>293.39999999999998</v>
       </c>
       <c r="AO4" t="s">
         <v>7</v>
@@ -7061,7 +7041,7 @@
         <v>1</v>
       </c>
       <c r="AQ4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AR4" t="s">
         <v>3</v>
@@ -7073,7 +7053,7 @@
         <v>5</v>
       </c>
       <c r="AU4" s="1">
-        <v>625.6</v>
+        <v>620.70000000000005</v>
       </c>
       <c r="AX4" t="s">
         <v>7</v>
@@ -7124,13 +7104,13 @@
         <v>14</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L5" t="s">
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N5" t="s">
         <v>3</v>
@@ -7142,7 +7122,7 @@
         <v>5</v>
       </c>
       <c r="Q5" s="1">
-        <v>3215.1</v>
+        <v>533.6</v>
       </c>
       <c r="U5" t="s">
         <v>7</v>
@@ -7172,7 +7152,7 @@
         <v>1</v>
       </c>
       <c r="AG5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AH5" t="s">
         <v>3</v>
@@ -7184,7 +7164,7 @@
         <v>5</v>
       </c>
       <c r="AK5" s="1">
-        <v>625.6</v>
+        <v>1159.2</v>
       </c>
       <c r="AO5" t="s">
         <v>7</v>
@@ -7193,7 +7173,7 @@
         <v>1</v>
       </c>
       <c r="AQ5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AR5" t="s">
         <v>3</v>
@@ -7205,7 +7185,7 @@
         <v>5</v>
       </c>
       <c r="AU5" s="1">
-        <v>533.6</v>
+        <v>538.5</v>
       </c>
       <c r="AX5" t="s">
         <v>10</v>
@@ -7262,7 +7242,7 @@
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N6" t="s">
         <v>3</v>
@@ -7274,7 +7254,7 @@
         <v>5</v>
       </c>
       <c r="Q6" s="1">
-        <v>111.9</v>
+        <v>1358.2</v>
       </c>
       <c r="U6" t="s">
         <v>7</v>
@@ -7298,13 +7278,13 @@
         <v>386.2</v>
       </c>
       <c r="AE6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AF6" t="s">
         <v>1</v>
       </c>
       <c r="AG6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AH6" t="s">
         <v>3</v>
@@ -7316,7 +7296,7 @@
         <v>5</v>
       </c>
       <c r="AK6" s="1">
-        <v>533.6</v>
+        <v>199</v>
       </c>
       <c r="AO6" t="s">
         <v>10</v>
@@ -7325,7 +7305,7 @@
         <v>1</v>
       </c>
       <c r="AQ6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="AR6" t="s">
         <v>3</v>
@@ -7337,7 +7317,7 @@
         <v>5</v>
       </c>
       <c r="AU6" s="1">
-        <v>1441.1</v>
+        <v>2594.4</v>
       </c>
       <c r="AX6" t="s">
         <v>11</v>
@@ -7388,13 +7368,13 @@
         <v>110</v>
       </c>
       <c r="K7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L7" t="s">
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="N7" t="s">
         <v>3</v>
@@ -7406,7 +7386,7 @@
         <v>5</v>
       </c>
       <c r="Q7" s="1">
-        <v>884.9</v>
+        <v>1968.8</v>
       </c>
       <c r="U7" t="s">
         <v>10</v>
@@ -7436,7 +7416,7 @@
         <v>1</v>
       </c>
       <c r="AG7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="AH7" t="s">
         <v>3</v>
@@ -7448,7 +7428,7 @@
         <v>5</v>
       </c>
       <c r="AK7" s="1">
-        <v>3327</v>
+        <v>2594.4</v>
       </c>
       <c r="AO7" t="s">
         <v>10</v>
@@ -7457,7 +7437,7 @@
         <v>1</v>
       </c>
       <c r="AQ7" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AR7" t="s">
         <v>3</v>
@@ -7469,7 +7449,7 @@
         <v>5</v>
       </c>
       <c r="AU7" s="1">
-        <v>1885.9</v>
+        <v>732.6</v>
       </c>
       <c r="AX7" t="s">
         <v>11</v>
@@ -7526,7 +7506,7 @@
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="N8" t="s">
         <v>3</v>
@@ -7538,7 +7518,7 @@
         <v>5</v>
       </c>
       <c r="Q8" s="1">
-        <v>469.1</v>
+        <v>1354</v>
       </c>
       <c r="U8" t="s">
         <v>11</v>
@@ -7562,13 +7542,13 @@
         <v>1354</v>
       </c>
       <c r="AE8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AF8" t="s">
         <v>1</v>
       </c>
       <c r="AG8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AH8" t="s">
         <v>3</v>
@@ -7580,7 +7560,7 @@
         <v>5</v>
       </c>
       <c r="AK8" s="1">
-        <v>1354</v>
+        <v>533.6</v>
       </c>
       <c r="AO8" t="s">
         <v>11</v>
@@ -7589,7 +7569,7 @@
         <v>1</v>
       </c>
       <c r="AQ8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="AR8" t="s">
         <v>3</v>
@@ -7601,7 +7581,7 @@
         <v>5</v>
       </c>
       <c r="AU8" s="1">
-        <v>82.9</v>
+        <v>820.4</v>
       </c>
       <c r="AX8" t="s">
         <v>11</v>
@@ -7694,7 +7674,7 @@
         <v>1346</v>
       </c>
       <c r="AE9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AF9" t="s">
         <v>1</v>
@@ -7712,7 +7692,7 @@
         <v>5</v>
       </c>
       <c r="AK9" s="1">
-        <v>1346</v>
+        <v>1354</v>
       </c>
       <c r="AO9" t="s">
         <v>11</v>
@@ -7721,7 +7701,7 @@
         <v>1</v>
       </c>
       <c r="AQ9" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AR9" t="s">
         <v>3</v>
@@ -7733,7 +7713,7 @@
         <v>5</v>
       </c>
       <c r="AU9" s="1">
-        <v>1271.0999999999999</v>
+        <v>533.6</v>
       </c>
       <c r="AX9" t="s">
         <v>12</v>
@@ -7826,7 +7806,7 @@
         <v>928</v>
       </c>
       <c r="AE10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF10" t="s">
         <v>1</v>
@@ -7844,7 +7824,7 @@
         <v>5</v>
       </c>
       <c r="AK10" s="1">
-        <v>928</v>
+        <v>1346</v>
       </c>
       <c r="AO10" t="s">
         <v>12</v>
@@ -7934,7 +7914,7 @@
         <v>5</v>
       </c>
       <c r="Q11" s="1">
-        <v>3169.6</v>
+        <v>1811.4</v>
       </c>
       <c r="U11" t="s">
         <v>14</v>
@@ -7955,16 +7935,16 @@
         <v>5</v>
       </c>
       <c r="AA11" s="1">
-        <v>3086.7</v>
+        <v>3169.6</v>
       </c>
       <c r="AE11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AF11" t="s">
         <v>1</v>
       </c>
       <c r="AG11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AH11" t="s">
         <v>3</v>
@@ -7976,7 +7956,7 @@
         <v>5</v>
       </c>
       <c r="AK11" s="1">
-        <v>3169.6</v>
+        <v>928</v>
       </c>
       <c r="AO11" t="s">
         <v>13</v>
@@ -8054,7 +8034,7 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="N12" t="s">
         <v>3</v>
@@ -8066,7 +8046,7 @@
         <v>5</v>
       </c>
       <c r="Q12" s="1">
-        <v>2594.4</v>
+        <v>2746</v>
       </c>
       <c r="U12" t="s">
         <v>14</v>
@@ -8087,7 +8067,7 @@
         <v>5</v>
       </c>
       <c r="AA12" s="1">
-        <v>2594.4</v>
+        <v>2511.5</v>
       </c>
       <c r="AE12" t="s">
         <v>14</v>
@@ -8096,7 +8076,7 @@
         <v>1</v>
       </c>
       <c r="AG12" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AH12" t="s">
         <v>3</v>
@@ -8108,7 +8088,7 @@
         <v>5</v>
       </c>
       <c r="AK12" s="1">
-        <v>2594.4</v>
+        <v>1728.5</v>
       </c>
       <c r="AO12" t="s">
         <v>14</v>
@@ -8129,7 +8109,7 @@
         <v>5</v>
       </c>
       <c r="AU12" s="1">
-        <v>1728.5</v>
+        <v>2548.9</v>
       </c>
       <c r="AX12" t="s">
         <v>14</v>
@@ -8186,7 +8166,7 @@
         <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N13" t="s">
         <v>3</v>
@@ -8198,7 +8178,7 @@
         <v>5</v>
       </c>
       <c r="Q13" s="1">
-        <v>64.5</v>
+        <v>1271.0999999999999</v>
       </c>
       <c r="U13" t="s">
         <v>14</v>
@@ -8228,7 +8208,7 @@
         <v>1</v>
       </c>
       <c r="AG13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AH13" t="s">
         <v>3</v>
@@ -8240,7 +8220,7 @@
         <v>5</v>
       </c>
       <c r="AK13" s="1">
-        <v>64.5</v>
+        <v>4100</v>
       </c>
       <c r="AO13" t="s">
         <v>14</v>
@@ -8261,7 +8241,7 @@
         <v>5</v>
       </c>
       <c r="AU13" s="1">
-        <v>4100</v>
+        <v>3279.6</v>
       </c>
       <c r="AX13" t="s">
         <v>14</v>
@@ -8366,7 +8346,7 @@
         <v>1</v>
       </c>
       <c r="AG14" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="AH14" t="s">
         <v>3</v>
@@ -8474,7 +8454,7 @@
         <v>5</v>
       </c>
       <c r="Q15" s="1">
-        <v>228.7</v>
+        <v>113.2</v>
       </c>
       <c r="U15" t="s">
         <v>17</v>
@@ -8738,7 +8718,7 @@
         <v>5</v>
       </c>
       <c r="Q17" s="1">
-        <v>280.10000000000002</v>
+        <v>395.6</v>
       </c>
       <c r="U17" t="s">
         <v>17</v>
@@ -8870,7 +8850,7 @@
         <v>5</v>
       </c>
       <c r="Q18" s="1">
-        <v>2714.5</v>
+        <v>2830</v>
       </c>
       <c r="U18" t="s">
         <v>18</v>
@@ -8912,7 +8892,7 @@
         <v>5</v>
       </c>
       <c r="AK18" s="1">
-        <v>2438.9</v>
+        <v>2714.5</v>
       </c>
       <c r="AO18" t="s">
         <v>18</v>
@@ -9002,7 +8982,7 @@
         <v>5</v>
       </c>
       <c r="Q19" s="1">
-        <v>2801</v>
+        <v>2685.5</v>
       </c>
       <c r="U19" t="s">
         <v>18</v>
@@ -9174,7 +9154,7 @@
         <v>5</v>
       </c>
       <c r="AK20" s="1">
-        <v>6760.1</v>
+        <v>6484.5</v>
       </c>
       <c r="AO20" t="s">
         <v>18</v>
@@ -9304,7 +9284,7 @@
         <v>5</v>
       </c>
       <c r="AK21" s="1">
-        <v>6113.9</v>
+        <v>6389.5</v>
       </c>
       <c r="AO21" t="s">
         <v>20</v>
@@ -9420,7 +9400,7 @@
         <v>5</v>
       </c>
       <c r="AK22" s="1">
-        <v>1338.1</v>
+        <v>1062.5</v>
       </c>
       <c r="AO22" t="s">
         <v>20</v>
@@ -9527,7 +9507,7 @@
         <v>5</v>
       </c>
       <c r="AA25" s="1">
-        <v>358.5</v>
+        <v>300.2</v>
       </c>
       <c r="AE25" t="s">
         <v>0</v>
@@ -9624,7 +9604,7 @@
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N26" t="s">
         <v>3</v>
@@ -9636,7 +9616,7 @@
         <v>5</v>
       </c>
       <c r="Q26" s="1">
-        <v>773</v>
+        <v>1159.2</v>
       </c>
       <c r="U26" t="s">
         <v>0</v>
@@ -9657,7 +9637,7 @@
         <v>5</v>
       </c>
       <c r="AA26" s="1">
-        <v>293.39999999999998</v>
+        <v>351.7</v>
       </c>
       <c r="AE26" t="s">
         <v>7</v>
@@ -9666,7 +9646,7 @@
         <v>1</v>
       </c>
       <c r="AG26" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="AH26" t="s">
         <v>3</v>
@@ -9687,7 +9667,7 @@
         <v>1</v>
       </c>
       <c r="AQ26" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AR26" t="s">
         <v>3</v>
@@ -9699,7 +9679,7 @@
         <v>5</v>
       </c>
       <c r="AU26" s="1">
-        <v>1159.2</v>
+        <v>533.6</v>
       </c>
       <c r="AX26" t="s">
         <v>7</v>
@@ -9748,13 +9728,13 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="N27" t="s">
         <v>3</v>
@@ -9766,7 +9746,7 @@
         <v>5</v>
       </c>
       <c r="Q27" s="1">
-        <v>386.2</v>
+        <v>2594.4</v>
       </c>
       <c r="U27" t="s">
         <v>7</v>
@@ -9811,13 +9791,13 @@
         <v>533.6</v>
       </c>
       <c r="AO27" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AP27" t="s">
         <v>1</v>
       </c>
       <c r="AQ27" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AR27" t="s">
         <v>3</v>
@@ -9829,7 +9809,7 @@
         <v>5</v>
       </c>
       <c r="AU27" s="1">
-        <v>1774</v>
+        <v>625.6</v>
       </c>
       <c r="AX27" t="s">
         <v>7</v>
@@ -9884,7 +9864,7 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N28" t="s">
         <v>3</v>
@@ -9896,7 +9876,7 @@
         <v>5</v>
       </c>
       <c r="Q28" s="1">
-        <v>3327</v>
+        <v>732.6</v>
       </c>
       <c r="U28" t="s">
         <v>7</v>
@@ -9938,7 +9918,7 @@
         <v>5</v>
       </c>
       <c r="AK28" s="1">
-        <v>732.6</v>
+        <v>1679.6</v>
       </c>
       <c r="AO28" t="s">
         <v>10</v>
@@ -9947,7 +9927,7 @@
         <v>1</v>
       </c>
       <c r="AQ28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AR28" t="s">
         <v>3</v>
@@ -9959,7 +9939,7 @@
         <v>5</v>
       </c>
       <c r="AU28" s="1">
-        <v>1553</v>
+        <v>732.6</v>
       </c>
       <c r="AX28" t="s">
         <v>7</v>
@@ -10026,7 +10006,7 @@
         <v>5</v>
       </c>
       <c r="Q29" s="1">
-        <v>1206.5999999999999</v>
+        <v>820.4</v>
       </c>
       <c r="U29" t="s">
         <v>10</v>
@@ -10056,7 +10036,7 @@
         <v>1</v>
       </c>
       <c r="AG29" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AH29" t="s">
         <v>3</v>
@@ -10068,10 +10048,10 @@
         <v>5</v>
       </c>
       <c r="AK29" s="1">
-        <v>2594.4</v>
+        <v>1647.4</v>
       </c>
       <c r="AO29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AP29" t="s">
         <v>1</v>
@@ -10089,7 +10069,7 @@
         <v>5</v>
       </c>
       <c r="AU29" s="1">
-        <v>820.4</v>
+        <v>2594.4</v>
       </c>
       <c r="AX29" t="s">
         <v>10</v>
@@ -10156,7 +10136,7 @@
         <v>5</v>
       </c>
       <c r="Q30" s="1">
-        <v>147.4</v>
+        <v>533.6</v>
       </c>
       <c r="U30" t="s">
         <v>11</v>
@@ -10207,7 +10187,7 @@
         <v>1</v>
       </c>
       <c r="AQ30" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AR30" t="s">
         <v>3</v>
@@ -10219,7 +10199,7 @@
         <v>5</v>
       </c>
       <c r="AU30" s="1">
-        <v>533.6</v>
+        <v>1354</v>
       </c>
       <c r="AX30" t="s">
         <v>11</v>
@@ -10404,7 +10384,7 @@
         <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N32" t="s">
         <v>3</v>
@@ -10416,7 +10396,7 @@
         <v>5</v>
       </c>
       <c r="Q32" s="1">
-        <v>928</v>
+        <v>244.4</v>
       </c>
       <c r="U32" t="s">
         <v>13</v>
@@ -10467,7 +10447,7 @@
         <v>1</v>
       </c>
       <c r="AQ32" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AR32" t="s">
         <v>3</v>
@@ -10479,7 +10459,7 @@
         <v>5</v>
       </c>
       <c r="AU32" s="1">
-        <v>928</v>
+        <v>332.2</v>
       </c>
       <c r="AX32" t="s">
         <v>13</v>
@@ -10528,13 +10508,13 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N33" t="s">
         <v>3</v>
@@ -10546,7 +10526,7 @@
         <v>5</v>
       </c>
       <c r="Q33" s="1">
-        <v>51.3</v>
+        <v>683.6</v>
       </c>
       <c r="U33" t="s">
         <v>17</v>
@@ -10567,7 +10547,7 @@
         <v>5</v>
       </c>
       <c r="AA33" s="1">
-        <v>51.3</v>
+        <v>56.6</v>
       </c>
       <c r="AE33" t="s">
         <v>17</v>
@@ -10591,13 +10571,13 @@
         <v>228.7</v>
       </c>
       <c r="AO33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="AP33" t="s">
         <v>1</v>
       </c>
       <c r="AQ33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AR33" t="s">
         <v>3</v>
@@ -10609,7 +10589,7 @@
         <v>5</v>
       </c>
       <c r="AU33" s="1">
-        <v>51.3</v>
+        <v>595.79999999999995</v>
       </c>
       <c r="AX33" t="s">
         <v>17</v>
@@ -10664,7 +10644,7 @@
         <v>1</v>
       </c>
       <c r="M34" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N34" t="s">
         <v>3</v>
@@ -10676,7 +10656,7 @@
         <v>5</v>
       </c>
       <c r="Q34" s="1">
-        <v>331.2</v>
+        <v>107.9</v>
       </c>
       <c r="U34" t="s">
         <v>17</v>
@@ -10727,7 +10707,7 @@
         <v>1</v>
       </c>
       <c r="AQ34" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AR34" t="s">
         <v>3</v>
@@ -10739,7 +10719,7 @@
         <v>5</v>
       </c>
       <c r="AU34" s="1">
-        <v>331.2</v>
+        <v>228.7</v>
       </c>
       <c r="AX34" t="s">
         <v>17</v>
@@ -10794,7 +10774,7 @@
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N35" t="s">
         <v>3</v>
@@ -10806,7 +10786,7 @@
         <v>5</v>
       </c>
       <c r="Q35" s="1">
-        <v>457.5</v>
+        <v>331.2</v>
       </c>
       <c r="U35" t="s">
         <v>17</v>
@@ -10827,7 +10807,7 @@
         <v>5</v>
       </c>
       <c r="AA35" s="1">
-        <v>457.5</v>
+        <v>452.2</v>
       </c>
       <c r="AE35" t="s">
         <v>17</v>
@@ -10857,7 +10837,7 @@
         <v>1</v>
       </c>
       <c r="AQ35" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AR35" t="s">
         <v>3</v>
@@ -10869,7 +10849,7 @@
         <v>5</v>
       </c>
       <c r="AU35" s="1">
-        <v>457.5</v>
+        <v>331.2</v>
       </c>
       <c r="AX35" t="s">
         <v>17</v>
@@ -10918,13 +10898,13 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N36" t="s">
         <v>3</v>
@@ -10936,7 +10916,7 @@
         <v>5</v>
       </c>
       <c r="Q36" s="1">
-        <v>2616.3000000000002</v>
+        <v>400.9</v>
       </c>
       <c r="U36" t="s">
         <v>18</v>
@@ -10957,7 +10937,7 @@
         <v>5</v>
       </c>
       <c r="AA36" s="1">
-        <v>2616.3000000000002</v>
+        <v>2669.3</v>
       </c>
       <c r="AE36" t="s">
         <v>18</v>
@@ -10981,13 +10961,13 @@
         <v>2438.9</v>
       </c>
       <c r="AO36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP36" t="s">
         <v>1</v>
       </c>
       <c r="AQ36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AR36" t="s">
         <v>3</v>
@@ -10999,7 +10979,7 @@
         <v>5</v>
       </c>
       <c r="AU36" s="1">
-        <v>2616.3000000000002</v>
+        <v>280.10000000000002</v>
       </c>
       <c r="AX36" t="s">
         <v>18</v>
@@ -11054,7 +11034,7 @@
         <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N37" t="s">
         <v>3</v>
@@ -11066,7 +11046,7 @@
         <v>5</v>
       </c>
       <c r="Q37" s="1">
-        <v>2623.6</v>
+        <v>2559.6999999999998</v>
       </c>
       <c r="U37" t="s">
         <v>18</v>
@@ -11087,7 +11067,7 @@
         <v>5</v>
       </c>
       <c r="AA37" s="1">
-        <v>2623.6</v>
+        <v>2570.6</v>
       </c>
       <c r="AE37" t="s">
         <v>18</v>
@@ -11117,7 +11097,7 @@
         <v>1</v>
       </c>
       <c r="AQ37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AR37" t="s">
         <v>3</v>
@@ -11129,7 +11109,7 @@
         <v>5</v>
       </c>
       <c r="AU37" s="1">
-        <v>2623.6</v>
+        <v>2438.9</v>
       </c>
       <c r="AX37" t="s">
         <v>18</v>
@@ -11184,7 +11164,7 @@
         <v>1</v>
       </c>
       <c r="M38" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="N38" t="s">
         <v>3</v>
@@ -11196,7 +11176,7 @@
         <v>5</v>
       </c>
       <c r="Q38" s="1">
-        <v>6760.1</v>
+        <v>2680.2</v>
       </c>
       <c r="U38" t="s">
         <v>18</v>
@@ -11247,7 +11227,7 @@
         <v>1</v>
       </c>
       <c r="AQ38" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AR38" t="s">
         <v>3</v>
@@ -11259,7 +11239,7 @@
         <v>5</v>
       </c>
       <c r="AU38" s="1">
-        <v>6760.1</v>
+        <v>2801</v>
       </c>
       <c r="AX38" t="s">
         <v>18</v>
@@ -11308,7 +11288,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>1</v>
@@ -11326,7 +11306,7 @@
         <v>5</v>
       </c>
       <c r="Q39" s="1">
-        <v>6113.9</v>
+        <v>6760.1</v>
       </c>
       <c r="U39" t="s">
         <v>20</v>
@@ -11371,7 +11351,7 @@
         <v>6113.9</v>
       </c>
       <c r="AO39" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AP39" t="s">
         <v>1</v>
@@ -11389,7 +11369,7 @@
         <v>5</v>
       </c>
       <c r="AU39" s="1">
-        <v>6113.9</v>
+        <v>6760.1</v>
       </c>
       <c r="AX39" t="s">
         <v>20</v>
@@ -11444,7 +11424,7 @@
         <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N40" t="s">
         <v>3</v>
@@ -11456,7 +11436,7 @@
         <v>5</v>
       </c>
       <c r="Q40" s="1">
-        <v>1338.1</v>
+        <v>6113.9</v>
       </c>
       <c r="U40" t="s">
         <v>20</v>
@@ -11507,7 +11487,7 @@
         <v>1</v>
       </c>
       <c r="AQ40" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AR40" t="s">
         <v>3</v>
@@ -11519,7 +11499,7 @@
         <v>5</v>
       </c>
       <c r="AU40" s="1">
-        <v>1338.1</v>
+        <v>6113.9</v>
       </c>
       <c r="AX40" t="s">
         <v>20</v>
@@ -11568,13 +11548,13 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M41" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="N41" t="s">
         <v>3</v>
@@ -11586,7 +11566,7 @@
         <v>5</v>
       </c>
       <c r="Q41" s="1">
-        <v>1586.7</v>
+        <v>1338.1</v>
       </c>
       <c r="U41" t="s">
         <v>14</v>
@@ -11628,16 +11608,16 @@
         <v>5</v>
       </c>
       <c r="AK41" s="1">
-        <v>2060.6999999999998</v>
+        <v>1113.7</v>
       </c>
       <c r="AO41" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AP41" t="s">
         <v>1</v>
       </c>
       <c r="AQ41" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="AR41" t="s">
         <v>3</v>
@@ -11649,7 +11629,7 @@
         <v>5</v>
       </c>
       <c r="AU41" s="1">
-        <v>1634.1</v>
+        <v>1338.1</v>
       </c>
       <c r="AX41" t="s">
         <v>14</v>
@@ -11704,7 +11684,7 @@
         <v>1</v>
       </c>
       <c r="M42" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="N42" t="s">
         <v>3</v>
@@ -11716,7 +11696,7 @@
         <v>5</v>
       </c>
       <c r="Q42" s="1">
-        <v>2594.4</v>
+        <v>1728.5</v>
       </c>
       <c r="U42" t="s">
         <v>14</v>
@@ -11746,7 +11726,7 @@
         <v>1</v>
       </c>
       <c r="AG42" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="AH42" t="s">
         <v>3</v>
@@ -11758,7 +11738,7 @@
         <v>5</v>
       </c>
       <c r="AK42" s="1">
-        <v>2120.4</v>
+        <v>1968.8</v>
       </c>
       <c r="AO42" t="s">
         <v>14</v>
@@ -11767,7 +11747,7 @@
         <v>1</v>
       </c>
       <c r="AQ42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AR42" t="s">
         <v>3</v>
@@ -11779,7 +11759,7 @@
         <v>5</v>
       </c>
       <c r="AU42" s="1">
-        <v>4100</v>
+        <v>1728.5</v>
       </c>
       <c r="AX42" t="s">
         <v>14</v>
@@ -11832,7 +11812,7 @@
         <v>1</v>
       </c>
       <c r="M43" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N43" t="s">
         <v>3</v>
@@ -11844,7 +11824,7 @@
         <v>5</v>
       </c>
       <c r="Q43" s="1">
-        <v>1647.4</v>
+        <v>4100</v>
       </c>
       <c r="U43" t="s">
         <v>14</v>
@@ -11874,7 +11854,7 @@
         <v>1</v>
       </c>
       <c r="AG43" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AH43" t="s">
         <v>3</v>
@@ -11886,7 +11866,7 @@
         <v>5</v>
       </c>
       <c r="AK43" s="1">
-        <v>1647.4</v>
+        <v>2746</v>
       </c>
       <c r="AO43" t="s">
         <v>14</v>
@@ -11895,7 +11875,7 @@
         <v>1</v>
       </c>
       <c r="AQ43" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AR43" t="s">
         <v>3</v>
@@ -11907,7 +11887,7 @@
         <v>5</v>
       </c>
       <c r="AU43" s="1">
-        <v>94.4</v>
+        <v>4100</v>
       </c>
       <c r="AX43" t="s">
         <v>14</v>
@@ -11967,7 +11947,7 @@
       </c>
       <c r="AF45" s="1">
         <f>SUMIF(AE$3:AE$22,AE45,AK$3:AK$22)</f>
-        <v>651.90000000000009</v>
+        <v>651.9</v>
       </c>
       <c r="AG45" s="1">
         <f>SUMIF(AE$25:AE$44,AE45,AK$25:AK$44)</f>
@@ -11975,7 +11955,7 @@
       </c>
       <c r="AK45" s="1">
         <f>ABS(AF45-AG45)</f>
-        <v>1.1368683772161603E-13</v>
+        <v>0</v>
       </c>
       <c r="AO45" t="s">
         <v>0</v>
@@ -12764,7 +12744,7 @@
       </c>
       <c r="L55" s="1">
         <f>SUMIF(M$3:M$22,K55,Q$3:Q$22)</f>
-        <v>6112.7999999999993</v>
+        <v>6112.8</v>
       </c>
       <c r="M55" s="1">
         <f>SUMIF(M$25:M$44,K55,Q$25:Q$44)</f>
@@ -12772,7 +12752,7 @@
       </c>
       <c r="Q55" s="1">
         <f t="shared" si="5"/>
-        <v>9.0949470177292824E-13</v>
+        <v>0</v>
       </c>
       <c r="U55" t="s">
         <v>8</v>
@@ -12794,7 +12774,7 @@
       </c>
       <c r="AF55" s="1">
         <f>SUMIF(AG$3:AG$22,AE55,AK$3:AK$22)</f>
-        <v>6112.7999999999993</v>
+        <v>6112.8</v>
       </c>
       <c r="AG55" s="1">
         <f>SUMIF(AG$25:AG$44,AE55,AK$25:AK$44)</f>
@@ -12802,18 +12782,18 @@
       </c>
       <c r="AK55" s="1">
         <f t="shared" si="11"/>
-        <v>9.0949470177292824E-13</v>
+        <v>0</v>
       </c>
       <c r="AO55" t="s">
         <v>8</v>
       </c>
       <c r="AP55" s="1">
         <f>SUMIF(AQ$3:AQ$22,AO55,AU$3:AU$22)</f>
-        <v>6112.7999999999993</v>
+        <v>6112.8</v>
       </c>
       <c r="AQ55" s="1">
         <f>SUMIF(AQ$25:AQ$44,AO55,AU$25:AU$44)</f>
-        <v>6112.7999999999993</v>
+        <v>6112.8</v>
       </c>
       <c r="AU55" s="1">
         <f t="shared" si="14"/>
@@ -13435,8 +13415,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BD45:BD61 AU45:AU61 AK45:AK61 AA45:AA61 Q45:Q61">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="Q45:Q61 AA45:AA61 AK45:AK61 AU45:AU61 BD45:BD61">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
       <formula>100000000</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update model-2 log mean temperature difference calculation
</commit_message>
<xml_diff>
--- a/hens/test_case.xlsx
+++ b/hens/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\may3r\PycharmProjects\COSMO\hens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D4C4A7-193B-4D49-A7F6-BA9073886DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB322D1D-4088-46B2-93CA-56E128E7DE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19118" yWindow="0" windowWidth="19365" windowHeight="20963" xr2:uid="{55A3D58C-627B-4C9F-A3AC-B99D6961FBEF}"/>
   </bookViews>
@@ -6797,8 +6797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D46D52-B92F-4C13-90EE-CFC876B09C87}">
   <dimension ref="A2:BD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP68" sqref="AP68"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.4"/>
@@ -6874,7 +6874,7 @@
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="X3" t="s">
         <v>3</v>
@@ -7935,7 +7935,7 @@
         <v>5</v>
       </c>
       <c r="AA11" s="1">
-        <v>3169.6</v>
+        <v>3086.7</v>
       </c>
       <c r="AE11" t="s">
         <v>13</v>
@@ -8067,7 +8067,7 @@
         <v>5</v>
       </c>
       <c r="AA12" s="1">
-        <v>2511.5</v>
+        <v>2594.4</v>
       </c>
       <c r="AE12" t="s">
         <v>14</v>
@@ -8322,7 +8322,7 @@
         <v>1</v>
       </c>
       <c r="W14" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="X14" t="s">
         <v>3</v>
@@ -8871,7 +8871,7 @@
         <v>5</v>
       </c>
       <c r="AA18" s="1">
-        <v>2438.9</v>
+        <v>2714.5</v>
       </c>
       <c r="AE18" t="s">
         <v>18</v>
@@ -9133,7 +9133,7 @@
         <v>5</v>
       </c>
       <c r="AA20" s="1">
-        <v>6760.1</v>
+        <v>6484.5</v>
       </c>
       <c r="AE20" t="s">
         <v>18</v>
@@ -9263,7 +9263,7 @@
         <v>5</v>
       </c>
       <c r="AA21" s="1">
-        <v>6113.9</v>
+        <v>6389.5</v>
       </c>
       <c r="AE21" t="s">
         <v>20</v>
@@ -9379,7 +9379,7 @@
         <v>5</v>
       </c>
       <c r="AA22" s="1">
-        <v>1338.1</v>
+        <v>1062.5</v>
       </c>
       <c r="AE22" t="s">
         <v>20</v>
@@ -9507,7 +9507,7 @@
         <v>5</v>
       </c>
       <c r="AA25" s="1">
-        <v>300.2</v>
+        <v>347.9</v>
       </c>
       <c r="AE25" t="s">
         <v>0</v>
@@ -9637,7 +9637,7 @@
         <v>5</v>
       </c>
       <c r="AA26" s="1">
-        <v>351.7</v>
+        <v>304</v>
       </c>
       <c r="AE26" t="s">
         <v>7</v>
@@ -10547,7 +10547,7 @@
         <v>5</v>
       </c>
       <c r="AA33" s="1">
-        <v>56.6</v>
+        <v>113.2</v>
       </c>
       <c r="AE33" t="s">
         <v>17</v>
@@ -10807,7 +10807,7 @@
         <v>5</v>
       </c>
       <c r="AA35" s="1">
-        <v>452.2</v>
+        <v>395.6</v>
       </c>
       <c r="AE35" t="s">
         <v>17</v>
@@ -10937,7 +10937,7 @@
         <v>5</v>
       </c>
       <c r="AA36" s="1">
-        <v>2669.3</v>
+        <v>2565</v>
       </c>
       <c r="AE36" t="s">
         <v>18</v>
@@ -11067,7 +11067,7 @@
         <v>5</v>
       </c>
       <c r="AA37" s="1">
-        <v>2570.6</v>
+        <v>2674.9</v>
       </c>
       <c r="AE37" t="s">
         <v>18</v>
@@ -12763,11 +12763,11 @@
       </c>
       <c r="W55" s="1">
         <f>SUMIF(W$25:W$44,U55,AA$25:AA$44)</f>
-        <v>6112.8</v>
+        <v>6112.7999999999993</v>
       </c>
       <c r="AA55" s="1">
         <f t="shared" si="8"/>
-        <v>9.0949470177292824E-13</v>
+        <v>0</v>
       </c>
       <c r="AE55" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add model-6, the combined model
</commit_message>
<xml_diff>
--- a/hens/test_case.xlsx
+++ b/hens/test_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\may3r\PycharmProjects\COSMO\hens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB322D1D-4088-46B2-93CA-56E128E7DE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155637E0-E3F5-4DF1-B26F-4A0690568928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19118" yWindow="0" windowWidth="19365" windowHeight="20963" xr2:uid="{55A3D58C-627B-4C9F-A3AC-B99D6961FBEF}"/>
+    <workbookView xWindow="6713" yWindow="1837" windowWidth="30044" windowHeight="17093" xr2:uid="{55A3D58C-627B-4C9F-A3AC-B99D6961FBEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="106">
   <si>
     <t>HS1</t>
   </si>
@@ -400,6 +400,9 @@
   <si>
     <t>Hot</t>
   </si>
+  <si>
+    <t>M6</t>
+  </si>
 </sst>
 </file>
 
@@ -583,7 +586,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{3A896AD7-4125-4BEC-87EF-D4193813A363}"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -6440,12 +6453,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E70EA7A-D1DD-4AB3-B1A7-7C3340032068}" name="Table3" displayName="Table3" ref="A2:F22" totalsRowShown="0">
   <autoFilter ref="A2:F22" xr:uid="{5282843C-0FDD-C940-ABEB-01C7BA357338}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{51161E5C-B970-4A5B-8104-33DD52FA0EF6}" name="Stream no" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{51161E5C-B970-4A5B-8104-33DD52FA0EF6}" name="Stream no" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{71E0C6C2-353E-41AC-B4DB-82579879651E}" name="Stream Name"/>
-    <tableColumn id="3" xr3:uid="{BAED1916-3B93-426B-8D2C-3C3D00DDDA30}" name="Supply Temp" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{F2FA5C5B-2BC4-4460-8649-C7005BB98E94}" name="Target Temp" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{4EC3CF15-387C-4C65-832E-C5CEE8106FE1}" name="Heat Cap" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{FDD9F0D0-850A-4715-B314-5C921BF0C69A}" name="Enthalpy change" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{BAED1916-3B93-426B-8D2C-3C3D00DDDA30}" name="Supply Temp" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{F2FA5C5B-2BC4-4460-8649-C7005BB98E94}" name="Target Temp" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{4EC3CF15-387C-4C65-832E-C5CEE8106FE1}" name="Heat Cap" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{FDD9F0D0-850A-4715-B314-5C921BF0C69A}" name="Enthalpy change" dataDxfId="7">
       <calculatedColumnFormula>IF(Table3[[#This Row],[Heat Cap]],ABS(Table3[[#This Row],[Target Temp]]-Table3[[#This Row],[Supply Temp]])*Table3[[#This Row],[Heat Cap]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6457,12 +6470,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09A6D4DF-E638-4138-8EF0-4D8D308F4C4E}" name="Table4" displayName="Table4" ref="H2:M22" totalsRowShown="0">
   <autoFilter ref="H2:M22" xr:uid="{C2819A13-B954-F744-A937-195205D73C92}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{ECA15CAA-9B7C-4CA8-9A92-76A96085E693}" name="Stream no" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{ECA15CAA-9B7C-4CA8-9A92-76A96085E693}" name="Stream no" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{C7FD695F-4DD9-480C-9BE7-CBF936487862}" name="Stream Name"/>
-    <tableColumn id="3" xr3:uid="{6B08F010-5BE0-469A-AFEC-401DEFAC2BC2}" name="Supply Temp" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{6DAB91F0-ABCB-4103-A612-B4CB15012200}" name="Target Temp" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{9C848C1C-BC49-4229-916A-1B024467F3FA}" name="Heat Cap" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{CB901371-BCA9-417B-9021-899661F2CBCF}" name="Enthalpy change" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{6B08F010-5BE0-469A-AFEC-401DEFAC2BC2}" name="Supply Temp" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{6DAB91F0-ABCB-4103-A612-B4CB15012200}" name="Target Temp" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{9C848C1C-BC49-4229-916A-1B024467F3FA}" name="Heat Cap" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{CB901371-BCA9-417B-9021-899661F2CBCF}" name="Enthalpy change" dataDxfId="2">
       <calculatedColumnFormula>IF(Table4[[#This Row],[Heat Cap]],ABS(Table4[[#This Row],[Target Temp]]-Table4[[#This Row],[Supply Temp]])*Table4[[#This Row],[Heat Cap]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6795,10 +6808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D46D52-B92F-4C13-90EE-CFC876B09C87}">
-  <dimension ref="A2:BD72"/>
+  <dimension ref="A2:BM72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC32" sqref="AC32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BQ36" sqref="BQ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.4"/>
@@ -6817,9 +6830,11 @@
     <col min="45" max="46" width="1.75" customWidth="1"/>
     <col min="53" max="53" width="1.33203125" bestFit="1" customWidth="1"/>
     <col min="54" max="55" width="1.75" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="1.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="1.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.4">
       <c r="K2" t="s">
         <v>27</v>
       </c>
@@ -6835,8 +6850,11 @@
       <c r="AX2" t="s">
         <v>30</v>
       </c>
+      <c r="BG2" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>15</v>
       </c>
@@ -6960,8 +6978,29 @@
       <c r="BD3" s="1">
         <v>376.3</v>
       </c>
+      <c r="BG3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM3" s="1">
+        <v>376.3</v>
+      </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -7076,8 +7115,29 @@
       <c r="BD4" s="1">
         <v>1159.2</v>
       </c>
+      <c r="BG4" t="s">
+        <v>7</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM4" s="1">
+        <v>1159.2</v>
+      </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -7208,8 +7268,29 @@
       <c r="BD5" s="1">
         <v>3327</v>
       </c>
+      <c r="BG5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>15</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM5" s="1">
+        <v>2594.4</v>
+      </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -7340,8 +7421,29 @@
       <c r="BD6" s="1">
         <v>469.1</v>
       </c>
+      <c r="BG6" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM6" s="1">
+        <v>732.6</v>
+      </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -7472,8 +7574,29 @@
       <c r="BD7" s="1">
         <v>773</v>
       </c>
+      <c r="BG7" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM7" s="1">
+        <v>708.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -7604,8 +7727,29 @@
       <c r="BD8" s="1">
         <v>111.9</v>
       </c>
+      <c r="BG8" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL8" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM8" s="1">
+        <v>157.30000000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -7736,8 +7880,29 @@
       <c r="BD9" s="1">
         <v>1346</v>
       </c>
+      <c r="BG9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM9" s="1">
+        <v>488.2</v>
+      </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -7868,8 +8033,29 @@
       <c r="BD10" s="1">
         <v>928</v>
       </c>
+      <c r="BG10" t="s">
+        <v>12</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM10" s="1">
+        <v>1346</v>
+      </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -8000,8 +8186,29 @@
       <c r="BD11" s="1">
         <v>2700.5</v>
       </c>
+      <c r="BG11" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH11" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM11" s="1">
+        <v>928</v>
+      </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -8132,8 +8339,29 @@
       <c r="BD12" s="1">
         <v>2594.4</v>
       </c>
+      <c r="BG12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI12" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK12" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL12" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM12" s="1">
+        <v>3169.6</v>
+      </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -8264,8 +8492,29 @@
       <c r="BD13" s="1">
         <v>533.6</v>
       </c>
+      <c r="BG13" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI13" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ13" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM13" s="1">
+        <v>2658.9</v>
+      </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -8408,8 +8657,29 @@
       <c r="BD14" s="1">
         <v>275.60000000000002</v>
       </c>
+      <c r="BG14" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH14" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK14" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM14" s="1">
+        <v>275.60000000000002</v>
+      </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -8540,8 +8810,29 @@
       <c r="BD15" s="1">
         <v>56.6</v>
       </c>
+      <c r="BG15" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ15" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK15" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL15" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM15" s="1">
+        <v>228.7</v>
+      </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -8672,8 +8963,29 @@
       <c r="BD16" s="1">
         <v>331.2</v>
       </c>
+      <c r="BG16" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ16" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL16" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM16" s="1">
+        <v>331.2</v>
+      </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -8804,8 +9116,29 @@
       <c r="BD17" s="1">
         <v>452.2</v>
       </c>
+      <c r="BG17" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH17" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ17" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK17" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL17" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM17" s="1">
+        <v>280.10000000000002</v>
+      </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -8936,8 +9269,29 @@
       <c r="BD18" s="1">
         <v>2886.6</v>
       </c>
+      <c r="BG18" t="s">
+        <v>18</v>
+      </c>
+      <c r="BH18" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ18" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK18" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL18" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM18" s="1">
+        <v>2714.5</v>
+      </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -9068,8 +9422,29 @@
       <c r="BD19" s="1">
         <v>2628.9</v>
       </c>
+      <c r="BG19" t="s">
+        <v>18</v>
+      </c>
+      <c r="BH19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI19" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ19" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK19" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL19" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM19" s="1">
+        <v>2801</v>
+      </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -9198,8 +9573,29 @@
       <c r="BD20" s="1">
         <v>6484.5</v>
       </c>
+      <c r="BG20" t="s">
+        <v>18</v>
+      </c>
+      <c r="BH20" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI20" t="s">
+        <v>19</v>
+      </c>
+      <c r="BJ20" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK20" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL20" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM20" s="1">
+        <v>6484.5</v>
+      </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -9328,8 +9724,29 @@
       <c r="BD21" s="1">
         <v>6389.5</v>
       </c>
+      <c r="BG21" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH21" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI21" t="s">
+        <v>19</v>
+      </c>
+      <c r="BJ21" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK21" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL21" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM21" s="1">
+        <v>6389.5</v>
+      </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -9444,8 +9861,29 @@
       <c r="BD22" s="1">
         <v>1062.5</v>
       </c>
+      <c r="BG22" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH22" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI22" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ22" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK22" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL22" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM22" s="1">
+        <v>1062.5</v>
+      </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -9572,8 +10010,29 @@
       <c r="BD25" s="1">
         <v>651.9</v>
       </c>
+      <c r="BG25" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH25" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI25" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ25" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK25" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL25" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM25" s="1">
+        <v>651.9</v>
+      </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -9702,8 +10161,29 @@
       <c r="BD26" s="1">
         <v>92.8</v>
       </c>
+      <c r="BG26" t="s">
+        <v>7</v>
+      </c>
+      <c r="BH26" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI26" t="s">
+        <v>15</v>
+      </c>
+      <c r="BJ26" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK26" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL26" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM26" s="1">
+        <v>332.2</v>
+      </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -9832,8 +10312,29 @@
       <c r="BD27" s="1">
         <v>773</v>
       </c>
+      <c r="BG27" t="s">
+        <v>7</v>
+      </c>
+      <c r="BH27" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI27" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ27" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK27" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL27" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM27" s="1">
+        <v>533.6</v>
+      </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -9962,8 +10463,29 @@
       <c r="BD28" s="1">
         <v>293.39999999999998</v>
       </c>
+      <c r="BG28" t="s">
+        <v>7</v>
+      </c>
+      <c r="BH28" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI28" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ28" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK28" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL28" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM28" s="1">
+        <v>293.39999999999998</v>
+      </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -10092,8 +10614,29 @@
       <c r="BD29" s="1">
         <v>3327</v>
       </c>
+      <c r="BG29" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH29" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI29" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ29" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK29" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL29" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM29" s="1">
+        <v>3327</v>
+      </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -10222,8 +10765,29 @@
       <c r="BD30" s="1">
         <v>1354</v>
       </c>
+      <c r="BG30" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH30" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI30" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ30" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK30" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL30" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM30" s="1">
+        <v>1354</v>
+      </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -10352,8 +10916,29 @@
       <c r="BD31" s="1">
         <v>1346</v>
       </c>
+      <c r="BG31" t="s">
+        <v>12</v>
+      </c>
+      <c r="BH31" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI31" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ31" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK31" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL31" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM31" s="1">
+        <v>1346</v>
+      </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -10482,8 +11067,29 @@
       <c r="BD32" s="1">
         <v>928</v>
       </c>
+      <c r="BG32" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH32" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI32" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ32" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK32" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL32" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM32" s="1">
+        <v>928</v>
+      </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -10612,8 +11218,29 @@
       <c r="BD33" s="1">
         <v>56.6</v>
       </c>
+      <c r="BG33" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH33" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI33" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ33" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK33" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL33" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM33" s="1">
+        <v>228.7</v>
+      </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -10742,8 +11369,29 @@
       <c r="BD34" s="1">
         <v>331.2</v>
       </c>
+      <c r="BG34" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH34" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI34" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ34" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK34" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL34" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM34" s="1">
+        <v>331.2</v>
+      </c>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -10872,8 +11520,29 @@
       <c r="BD35" s="1">
         <v>452.2</v>
       </c>
+      <c r="BG35" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH35" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI35" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ35" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK35" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL35" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM35" s="1">
+        <v>280.10000000000002</v>
+      </c>
     </row>
-    <row r="36" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -11002,8 +11671,29 @@
       <c r="BD36" s="1">
         <v>2611</v>
       </c>
+      <c r="BG36" t="s">
+        <v>18</v>
+      </c>
+      <c r="BH36" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI36" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ36" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK36" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL36" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM36" s="1">
+        <v>2438.9</v>
+      </c>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -11132,8 +11822,29 @@
       <c r="BD37" s="1">
         <v>2628.9</v>
       </c>
+      <c r="BG37" t="s">
+        <v>18</v>
+      </c>
+      <c r="BH37" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI37" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ37" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK37" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL37" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM37" s="1">
+        <v>2801</v>
+      </c>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -11262,8 +11973,29 @@
       <c r="BD38" s="1">
         <v>6760.1</v>
       </c>
+      <c r="BG38" t="s">
+        <v>18</v>
+      </c>
+      <c r="BH38" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI38" t="s">
+        <v>19</v>
+      </c>
+      <c r="BJ38" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK38" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL38" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM38" s="1">
+        <v>6760.1</v>
+      </c>
     </row>
-    <row r="39" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -11392,8 +12124,29 @@
       <c r="BD39" s="1">
         <v>6113.9</v>
       </c>
+      <c r="BG39" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH39" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI39" t="s">
+        <v>19</v>
+      </c>
+      <c r="BJ39" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK39" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL39" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM39" s="1">
+        <v>6113.9</v>
+      </c>
     </row>
-    <row r="40" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -11522,8 +12275,29 @@
       <c r="BD40" s="1">
         <v>1338.1</v>
       </c>
+      <c r="BG40" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH40" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI40" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ40" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK40" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL40" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM40" s="1">
+        <v>1338.1</v>
+      </c>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -11652,8 +12426,29 @@
       <c r="BD41" s="1">
         <v>2700.5</v>
       </c>
+      <c r="BG41" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH41" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI41" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ41" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK41" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL41" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM41" s="1">
+        <v>2793.3</v>
+      </c>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -11782,8 +12577,29 @@
       <c r="BD42" s="1">
         <v>2594.4</v>
       </c>
+      <c r="BG42" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH42" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI42" t="s">
+        <v>15</v>
+      </c>
+      <c r="BJ42" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK42" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL42" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM42" s="1">
+        <v>2262.1999999999998</v>
+      </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -11910,8 +12726,29 @@
       <c r="BD43" s="1">
         <v>533.6</v>
       </c>
+      <c r="BG43" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH43" t="s">
+        <v>1</v>
+      </c>
+      <c r="BI43" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ43" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK43" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL43" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM43" s="1">
+        <v>773</v>
+      </c>
     </row>
-    <row r="45" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.4">
       <c r="K45" t="s">
         <v>0</v>
       </c>
@@ -11987,8 +12824,23 @@
         <f>ABS(AY45-AZ45)</f>
         <v>1.1368683772161603E-13</v>
       </c>
+      <c r="BG45" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH45" s="1">
+        <f>SUMIF(BG$3:BG$22,BG45,BM$3:BM$22)</f>
+        <v>651.90000000000009</v>
+      </c>
+      <c r="BI45" s="1">
+        <f>SUMIF(BG$25:BG$44,BG45,BM$25:BM$44)</f>
+        <v>651.9</v>
+      </c>
+      <c r="BM45" s="1">
+        <f>ABS(BH45-BI45)</f>
+        <v>1.1368683772161603E-13</v>
+      </c>
     </row>
-    <row r="46" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.4">
       <c r="K46" t="s">
         <v>7</v>
       </c>
@@ -12064,8 +12916,23 @@
         <f t="shared" ref="BD46:BD61" si="17">ABS(AY46-AZ46)</f>
         <v>2.2737367544323206E-13</v>
       </c>
+      <c r="BG46" t="s">
+        <v>7</v>
+      </c>
+      <c r="BH46" s="1">
+        <f t="shared" ref="BH46:BH54" si="18">SUMIF(BG$3:BG$22,BG46,BM$3:BM$22)</f>
+        <v>1159.2</v>
+      </c>
+      <c r="BI46" s="1">
+        <f t="shared" ref="BI46:BI54" si="19">SUMIF(BG$25:BG$44,BG46,BM$25:BM$44)</f>
+        <v>1159.1999999999998</v>
+      </c>
+      <c r="BM46" s="1">
+        <f t="shared" ref="BM46:BM61" si="20">ABS(BH46-BI46)</f>
+        <v>2.2737367544323206E-13</v>
+      </c>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:65" x14ac:dyDescent="0.4">
       <c r="K47" t="s">
         <v>10</v>
       </c>
@@ -12141,8 +13008,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG47" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH47" s="1">
+        <f t="shared" si="18"/>
+        <v>3327</v>
+      </c>
+      <c r="BI47" s="1">
+        <f t="shared" si="19"/>
+        <v>3327</v>
+      </c>
+      <c r="BM47" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -12225,8 +13107,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG48" t="s">
+        <v>11</v>
+      </c>
+      <c r="BH48" s="1">
+        <f t="shared" si="18"/>
+        <v>1354</v>
+      </c>
+      <c r="BI48" s="1">
+        <f t="shared" si="19"/>
+        <v>1354</v>
+      </c>
+      <c r="BM48" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A49" cm="1">
         <f t="array" ref="A49:A72">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.TOCOL(H5:I21)),,-1)</f>
         <v>150</v>
@@ -12310,8 +13207,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG49" t="s">
+        <v>12</v>
+      </c>
+      <c r="BH49" s="1">
+        <f t="shared" si="18"/>
+        <v>1346</v>
+      </c>
+      <c r="BI49" s="1">
+        <f t="shared" si="19"/>
+        <v>1346</v>
+      </c>
+      <c r="BM49" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>149</v>
       </c>
@@ -12394,8 +13306,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG50" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH50" s="1">
+        <f t="shared" si="18"/>
+        <v>928</v>
+      </c>
+      <c r="BI50" s="1">
+        <f t="shared" si="19"/>
+        <v>928</v>
+      </c>
+      <c r="BM50" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>137</v>
       </c>
@@ -12478,8 +13405,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG51" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH51" s="1">
+        <f t="shared" si="18"/>
+        <v>840</v>
+      </c>
+      <c r="BI51" s="1">
+        <f t="shared" si="19"/>
+        <v>840</v>
+      </c>
+      <c r="BM51" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>135</v>
       </c>
@@ -12562,8 +13504,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG52" t="s">
+        <v>18</v>
+      </c>
+      <c r="BH52" s="1">
+        <f t="shared" si="18"/>
+        <v>12000</v>
+      </c>
+      <c r="BI52" s="1">
+        <f t="shared" si="19"/>
+        <v>12000</v>
+      </c>
+      <c r="BM52" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>122</v>
       </c>
@@ -12646,8 +13603,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG53" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH53" s="1">
+        <f t="shared" si="18"/>
+        <v>7452</v>
+      </c>
+      <c r="BI53" s="1">
+        <f t="shared" si="19"/>
+        <v>7452</v>
+      </c>
+      <c r="BM53" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>111</v>
       </c>
@@ -12730,8 +13702,23 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG54" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH54" s="1">
+        <f t="shared" si="18"/>
+        <v>5828.5</v>
+      </c>
+      <c r="BI54" s="1">
+        <f t="shared" si="19"/>
+        <v>5828.5</v>
+      </c>
+      <c r="BM54" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>110</v>
       </c>
@@ -12814,8 +13801,23 @@
         <f t="shared" si="17"/>
         <v>9.0949470177292824E-13</v>
       </c>
+      <c r="BG55" t="s">
+        <v>8</v>
+      </c>
+      <c r="BH55" s="1">
+        <f>SUMIF(BI$3:BI$22,BG55,BM$3:BM$22)</f>
+        <v>6112.7999999999993</v>
+      </c>
+      <c r="BI55" s="1">
+        <f>SUMIF(BI$25:BI$44,BG55,BM$25:BM$44)</f>
+        <v>6112.8</v>
+      </c>
+      <c r="BM55" s="1">
+        <f t="shared" si="20"/>
+        <v>9.0949470177292824E-13</v>
+      </c>
     </row>
-    <row r="56" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>105</v>
       </c>
@@ -12827,11 +13829,11 @@
         <v>15</v>
       </c>
       <c r="L56" s="1">
-        <f t="shared" ref="L56:L61" si="18">SUMIF(M$3:M$22,K56,Q$3:Q$22)</f>
+        <f t="shared" ref="L56:L61" si="21">SUMIF(M$3:M$22,K56,Q$3:Q$22)</f>
         <v>2594.4</v>
       </c>
       <c r="M56" s="1">
-        <f t="shared" ref="M56:M61" si="19">SUMIF(M$25:M$44,K56,Q$25:Q$44)</f>
+        <f t="shared" ref="M56:M61" si="22">SUMIF(M$25:M$44,K56,Q$25:Q$44)</f>
         <v>2594.4</v>
       </c>
       <c r="Q56" s="1">
@@ -12842,11 +13844,11 @@
         <v>15</v>
       </c>
       <c r="V56" s="1">
-        <f t="shared" ref="V56:V61" si="20">SUMIF(W$3:W$22,U56,AA$3:AA$22)</f>
+        <f t="shared" ref="V56:V61" si="23">SUMIF(W$3:W$22,U56,AA$3:AA$22)</f>
         <v>2594.4</v>
       </c>
       <c r="W56" s="1">
-        <f t="shared" ref="W56:W61" si="21">SUMIF(W$25:W$44,U56,AA$25:AA$44)</f>
+        <f t="shared" ref="W56:W61" si="24">SUMIF(W$25:W$44,U56,AA$25:AA$44)</f>
         <v>2594.4</v>
       </c>
       <c r="AA56" s="1">
@@ -12857,11 +13859,11 @@
         <v>15</v>
       </c>
       <c r="AF56" s="1">
-        <f t="shared" ref="AF56:AF61" si="22">SUMIF(AG$3:AG$22,AE56,AK$3:AK$22)</f>
+        <f t="shared" ref="AF56:AF61" si="25">SUMIF(AG$3:AG$22,AE56,AK$3:AK$22)</f>
         <v>2594.4</v>
       </c>
       <c r="AG56" s="1">
-        <f t="shared" ref="AG56:AG61" si="23">SUMIF(AG$25:AG$44,AE56,AK$25:AK$44)</f>
+        <f t="shared" ref="AG56:AG61" si="26">SUMIF(AG$25:AG$44,AE56,AK$25:AK$44)</f>
         <v>2594.4</v>
       </c>
       <c r="AK56" s="1">
@@ -12872,11 +13874,11 @@
         <v>15</v>
       </c>
       <c r="AP56" s="1">
-        <f t="shared" ref="AP56:AP61" si="24">SUMIF(AQ$3:AQ$22,AO56,AU$3:AU$22)</f>
+        <f t="shared" ref="AP56:AP61" si="27">SUMIF(AQ$3:AQ$22,AO56,AU$3:AU$22)</f>
         <v>2594.4</v>
       </c>
       <c r="AQ56" s="1">
-        <f t="shared" ref="AQ56:AQ61" si="25">SUMIF(AQ$25:AQ$44,AO56,AU$25:AU$44)</f>
+        <f t="shared" ref="AQ56:AQ61" si="28">SUMIF(AQ$25:AQ$44,AO56,AU$25:AU$44)</f>
         <v>2594.4</v>
       </c>
       <c r="AU56" s="1">
@@ -12887,19 +13889,34 @@
         <v>15</v>
       </c>
       <c r="AY56" s="1">
-        <f t="shared" ref="AY56:AY61" si="26">SUMIF(AZ$3:AZ$22,AX56,BD$3:BD$22)</f>
+        <f t="shared" ref="AY56:AY61" si="29">SUMIF(AZ$3:AZ$22,AX56,BD$3:BD$22)</f>
         <v>2594.4</v>
       </c>
       <c r="AZ56" s="1">
-        <f t="shared" ref="AZ56:AZ61" si="27">SUMIF(AZ$25:AZ$44,AX56,BD$25:BD$44)</f>
+        <f t="shared" ref="AZ56:AZ61" si="30">SUMIF(AZ$25:AZ$44,AX56,BD$25:BD$44)</f>
         <v>2594.4</v>
       </c>
       <c r="BD56" s="1">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG56" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH56" s="1">
+        <f t="shared" ref="BH56:BH61" si="31">SUMIF(BI$3:BI$22,BG56,BM$3:BM$22)</f>
+        <v>2594.4</v>
+      </c>
+      <c r="BI56" s="1">
+        <f t="shared" ref="BI56:BI61" si="32">SUMIF(BI$25:BI$44,BG56,BM$25:BM$44)</f>
+        <v>2594.3999999999996</v>
+      </c>
+      <c r="BM56" s="1">
+        <f t="shared" si="20"/>
+        <v>4.5474735088646412E-13</v>
+      </c>
     </row>
-    <row r="57" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>100</v>
       </c>
@@ -12911,11 +13928,11 @@
         <v>9</v>
       </c>
       <c r="L57" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>4100</v>
       </c>
       <c r="M57" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>4100</v>
       </c>
       <c r="Q57" s="1">
@@ -12926,11 +13943,11 @@
         <v>9</v>
       </c>
       <c r="V57" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>4100</v>
       </c>
       <c r="W57" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>4100</v>
       </c>
       <c r="AA57" s="1">
@@ -12941,11 +13958,11 @@
         <v>9</v>
       </c>
       <c r="AF57" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>4100</v>
       </c>
       <c r="AG57" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>4100</v>
       </c>
       <c r="AK57" s="1">
@@ -12956,11 +13973,11 @@
         <v>9</v>
       </c>
       <c r="AP57" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>4100</v>
       </c>
       <c r="AQ57" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>4100</v>
       </c>
       <c r="AU57" s="1">
@@ -12971,19 +13988,34 @@
         <v>9</v>
       </c>
       <c r="AY57" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>4100</v>
       </c>
       <c r="AZ57" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>4100</v>
       </c>
       <c r="BD57" s="1">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG57" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH57" s="1">
+        <f t="shared" si="31"/>
+        <v>4100</v>
+      </c>
+      <c r="BI57" s="1">
+        <f t="shared" si="32"/>
+        <v>4100</v>
+      </c>
+      <c r="BM57" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>95</v>
       </c>
@@ -12995,11 +14027,11 @@
         <v>2</v>
       </c>
       <c r="L58" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>864.8</v>
       </c>
       <c r="M58" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>864.8</v>
       </c>
       <c r="Q58" s="1">
@@ -13010,11 +14042,11 @@
         <v>2</v>
       </c>
       <c r="V58" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>864.8</v>
       </c>
       <c r="W58" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>864.8</v>
       </c>
       <c r="AA58" s="1">
@@ -13025,11 +14057,11 @@
         <v>2</v>
       </c>
       <c r="AF58" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>864.8</v>
       </c>
       <c r="AG58" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>864.8</v>
       </c>
       <c r="AK58" s="1">
@@ -13040,11 +14072,11 @@
         <v>2</v>
       </c>
       <c r="AP58" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>864.8</v>
       </c>
       <c r="AQ58" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>864.8</v>
       </c>
       <c r="AU58" s="1">
@@ -13055,19 +14087,34 @@
         <v>2</v>
       </c>
       <c r="AY58" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>864.8</v>
       </c>
       <c r="AZ58" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>864.8</v>
       </c>
       <c r="BD58" s="1">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG58" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH58" s="1">
+        <f t="shared" si="31"/>
+        <v>864.8</v>
+      </c>
+      <c r="BI58" s="1">
+        <f t="shared" si="32"/>
+        <v>864.8</v>
+      </c>
+      <c r="BM58" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>86</v>
       </c>
@@ -13079,11 +14126,11 @@
         <v>6</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7002.5</v>
       </c>
       <c r="M59" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>7002.5</v>
       </c>
       <c r="Q59" s="1">
@@ -13094,11 +14141,11 @@
         <v>6</v>
       </c>
       <c r="V59" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>7002.5</v>
       </c>
       <c r="W59" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>7002.5</v>
       </c>
       <c r="AA59" s="1">
@@ -13109,11 +14156,11 @@
         <v>6</v>
       </c>
       <c r="AF59" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>7002.5</v>
       </c>
       <c r="AG59" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>7002.5</v>
       </c>
       <c r="AK59" s="1">
@@ -13124,11 +14171,11 @@
         <v>6</v>
       </c>
       <c r="AP59" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>7002.5</v>
       </c>
       <c r="AQ59" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>7002.5</v>
       </c>
       <c r="AU59" s="1">
@@ -13139,19 +14186,34 @@
         <v>6</v>
       </c>
       <c r="AY59" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>7002.5</v>
       </c>
       <c r="AZ59" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>7002.5</v>
       </c>
       <c r="BD59" s="1">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG59" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH59" s="1">
+        <f t="shared" si="31"/>
+        <v>7002.5</v>
+      </c>
+      <c r="BI59" s="1">
+        <f t="shared" si="32"/>
+        <v>7002.5</v>
+      </c>
+      <c r="BM59" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>80</v>
       </c>
@@ -13163,11 +14225,11 @@
         <v>19</v>
       </c>
       <c r="L60" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>12874</v>
       </c>
       <c r="M60" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>12874</v>
       </c>
       <c r="Q60" s="1">
@@ -13178,11 +14240,11 @@
         <v>19</v>
       </c>
       <c r="V60" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>12874</v>
       </c>
       <c r="W60" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>12874</v>
       </c>
       <c r="AA60" s="1">
@@ -13193,11 +14255,11 @@
         <v>19</v>
       </c>
       <c r="AF60" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>12874</v>
       </c>
       <c r="AG60" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>12874</v>
       </c>
       <c r="AK60" s="1">
@@ -13208,11 +14270,11 @@
         <v>19</v>
       </c>
       <c r="AP60" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>12874</v>
       </c>
       <c r="AQ60" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>12874</v>
       </c>
       <c r="AU60" s="1">
@@ -13223,19 +14285,34 @@
         <v>19</v>
       </c>
       <c r="AY60" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>12874</v>
       </c>
       <c r="AZ60" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>12874</v>
       </c>
       <c r="BD60" s="1">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG60" t="s">
+        <v>19</v>
+      </c>
+      <c r="BH60" s="1">
+        <f t="shared" si="31"/>
+        <v>12874</v>
+      </c>
+      <c r="BI60" s="1">
+        <f t="shared" si="32"/>
+        <v>12874</v>
+      </c>
+      <c r="BM60" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>76</v>
       </c>
@@ -13247,11 +14324,11 @@
         <v>16</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1338.1</v>
       </c>
       <c r="M61" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>1338.1</v>
       </c>
       <c r="Q61" s="1">
@@ -13262,11 +14339,11 @@
         <v>16</v>
       </c>
       <c r="V61" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1338.1</v>
       </c>
       <c r="W61" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>1338.1</v>
       </c>
       <c r="AA61" s="1">
@@ -13277,11 +14354,11 @@
         <v>16</v>
       </c>
       <c r="AF61" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>1338.1</v>
       </c>
       <c r="AG61" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>1338.1</v>
       </c>
       <c r="AK61" s="1">
@@ -13292,11 +14369,11 @@
         <v>16</v>
       </c>
       <c r="AP61" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>1338.1</v>
       </c>
       <c r="AQ61" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>1338.1</v>
       </c>
       <c r="AU61" s="1">
@@ -13307,19 +14384,34 @@
         <v>16</v>
       </c>
       <c r="AY61" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>1338.1</v>
       </c>
       <c r="AZ61" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>1338.1</v>
       </c>
       <c r="BD61" s="1">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
+      <c r="BG61" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH61" s="1">
+        <f t="shared" si="31"/>
+        <v>1338.1</v>
+      </c>
+      <c r="BI61" s="1">
+        <f t="shared" si="32"/>
+        <v>1338.1</v>
+      </c>
+      <c r="BM61" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>75</v>
       </c>
@@ -13328,7 +14420,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>74</v>
       </c>
@@ -13337,7 +14429,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:56" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>66</v>
       </c>
@@ -13416,6 +14508,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q45:Q61 AA45:AA61 AK45:AK61 AU45:AU61 BD45:BD61">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+      <formula>100000000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM45:BM61">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
       <formula>100000000</formula>
     </cfRule>

</xml_diff>

<commit_message>
add matching class to contain heat exchanger matching
</commit_message>
<xml_diff>
--- a/hens/test_case.xlsx
+++ b/hens/test_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\may3r\PycharmProjects\COSMO\hens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155637E0-E3F5-4DF1-B26F-4A0690568928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B14E34C-ED99-4833-9967-C094310BEB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6713" yWindow="1837" windowWidth="30044" windowHeight="17093" xr2:uid="{55A3D58C-627B-4C9F-A3AC-B99D6961FBEF}"/>
+    <workbookView xWindow="6713" yWindow="1837" windowWidth="30044" windowHeight="17093" activeTab="1" xr2:uid="{55A3D58C-627B-4C9F-A3AC-B99D6961FBEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6810,8 +6810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D46D52-B92F-4C13-90EE-CFC876B09C87}">
   <dimension ref="A2:BM72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BQ36" sqref="BQ36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AV27" sqref="AV27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.4"/>
@@ -14525,7 +14525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A32EF91-7074-4ADB-B73E-EB23F6A95110}">
   <dimension ref="A1:AN101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AH27" sqref="AH27"/>
     </sheetView>
   </sheetViews>

</xml_diff>